<commit_message>
Estimate serial interval w/ bootstrapping
</commit_message>
<xml_diff>
--- a/Output/Table 1 - summary stats.xlsx
+++ b/Output/Table 1 - summary stats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Town</t>
   </si>
@@ -48,7 +48,31 @@
     <t>Cumulative cases*</t>
   </si>
   <si>
-    <t>* Cases are diagnosed as people having both watery diarrhae</t>
+    <t>Oslo</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Stolkholm</t>
+  </si>
+  <si>
+    <t>St. Petersburg</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Olso report</t>
+  </si>
+  <si>
+    <t>p10 of karlskrona report</t>
+  </si>
+  <si>
+    <t>Karlskrona (Sweden)</t>
+  </si>
+  <si>
+    <t>Bulliten + "on vital statistics of Sweden" pg 129"</t>
   </si>
 </sst>
 </file>
@@ -57,8 +81,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="174" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="175" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -92,7 +116,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -131,13 +155,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -149,11 +213,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -457,125 +534,257 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="6" width="12.44140625" customWidth="1"/>
+    <col min="1" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="7" width="12.44140625" customWidth="1"/>
+    <col min="9" max="9" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="I1" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="2">
+        <v>1853</v>
+      </c>
+      <c r="C2" s="7">
         <v>138030</v>
       </c>
-      <c r="C2" s="7">
+      <c r="D2" s="7">
         <v>7219</v>
       </c>
-      <c r="D2" s="7">
+      <c r="E2" s="7">
         <v>4737</v>
       </c>
-      <c r="E2" s="9">
-        <f>C2/B2*100</f>
+      <c r="F2" s="9">
+        <f>D2/C2*100</f>
         <v>5.2300224588857498</v>
       </c>
-      <c r="F2" s="9">
-        <f>D2/B2*100</f>
+      <c r="G2" s="9">
+        <f>E2/C2*100</f>
         <v>3.4318626385568352</v>
       </c>
-      <c r="G2" s="3">
-        <f>D2/C2</f>
+      <c r="H2" s="3">
+        <f>E2/D2</f>
         <v>0.65618506718382053</v>
       </c>
+      <c r="I2" s="11"/>
     </row>
-    <row r="3" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="4">
+        <v>1853</v>
+      </c>
+      <c r="C3" s="8">
         <v>8621</v>
       </c>
-      <c r="C3" s="8">
+      <c r="D3" s="8">
         <v>759</v>
       </c>
-      <c r="D3" s="8">
+      <c r="E3" s="8">
         <v>409</v>
       </c>
-      <c r="E3" s="10">
-        <f t="shared" ref="E3:E4" si="0">C3/B3*100</f>
+      <c r="F3" s="10">
+        <f t="shared" ref="F3:F6" si="0">D3/C3*100</f>
         <v>8.8040830530100926</v>
       </c>
-      <c r="F3" s="10">
-        <f t="shared" ref="F3:F4" si="1">D3/B3*100</f>
+      <c r="G3" s="10">
+        <f t="shared" ref="G3:G8" si="1">E3/C3*100</f>
         <v>4.7442292077485213</v>
       </c>
-      <c r="G3" s="5">
-        <f t="shared" ref="G3:G4" si="2">D3/C3</f>
+      <c r="H3" s="5">
+        <f t="shared" ref="H3:H8" si="2">E3/D3</f>
         <v>0.53886693017127796</v>
       </c>
+      <c r="I3" s="11"/>
     </row>
-    <row r="4" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:9" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="19">
+        <v>1857</v>
+      </c>
+      <c r="C4" s="20">
         <v>2617</v>
       </c>
-      <c r="C4" s="8">
+      <c r="D4" s="20">
         <v>294</v>
       </c>
-      <c r="D4" s="8">
+      <c r="E4" s="20">
         <v>201</v>
       </c>
-      <c r="E4" s="10">
+      <c r="F4" s="21">
         <f t="shared" si="0"/>
         <v>11.23423767672908</v>
       </c>
-      <c r="F4" s="10">
+      <c r="G4" s="22">
         <f t="shared" si="1"/>
         <v>7.6805502483760026</v>
       </c>
-      <c r="G4" s="5">
+      <c r="H4" s="23">
         <f t="shared" si="2"/>
         <v>0.68367346938775508</v>
       </c>
+      <c r="I4" s="24"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
         <v>10</v>
+      </c>
+      <c r="B5" s="15">
+        <v>1853</v>
+      </c>
+      <c r="C5" s="16">
+        <v>48000</v>
+      </c>
+      <c r="D5" s="17">
+        <v>2453</v>
+      </c>
+      <c r="E5" s="17">
+        <v>1597</v>
+      </c>
+      <c r="F5" s="12">
+        <f t="shared" si="0"/>
+        <v>5.1104166666666666</v>
+      </c>
+      <c r="G5" s="12">
+        <f>E5/C5*100</f>
+        <v>3.3270833333333334</v>
+      </c>
+      <c r="H5" s="14">
+        <f t="shared" si="2"/>
+        <v>0.65103954341622505</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="15">
+        <v>1834</v>
+      </c>
+      <c r="C6" s="11">
+        <v>97952</v>
+      </c>
+      <c r="D6" s="11">
+        <v>7906</v>
+      </c>
+      <c r="E6" s="17">
+        <v>3284</v>
+      </c>
+      <c r="F6" s="12">
+        <f t="shared" si="0"/>
+        <v>8.0713002286834374</v>
+      </c>
+      <c r="G6" s="12">
+        <f>E6/C6*100</f>
+        <v>3.3526625285854297</v>
+      </c>
+      <c r="H6" s="14">
+        <f t="shared" si="2"/>
+        <v>0.41538072350113836</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="15">
+        <v>1852</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="17">
+        <v>13504</v>
+      </c>
+      <c r="E7" s="17">
+        <v>5333</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="14">
+        <f t="shared" si="2"/>
+        <v>0.39492002369668244</v>
+      </c>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="15">
+        <v>1853</v>
+      </c>
+      <c r="C8" s="18">
+        <v>11378</v>
+      </c>
+      <c r="D8" s="11">
+        <v>1925</v>
+      </c>
+      <c r="E8" s="17">
+        <v>1055</v>
+      </c>
+      <c r="F8" s="12">
+        <f>D8/C8*100</f>
+        <v>16.918614870803307</v>
+      </c>
+      <c r="G8" s="12">
+        <f t="shared" si="1"/>
+        <v>9.2722798382844083</v>
+      </c>
+      <c r="H8" s="14">
+        <f t="shared" si="2"/>
+        <v>0.54805194805194801</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add all-cause monthly mort for CPH and all other cities
Faceted plots with differering colors and linetypes
</commit_message>
<xml_diff>
--- a/Output/Table 1 - summary stats.xlsx
+++ b/Output/Table 1 - summary stats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>Town</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>Bulliten + "on vital statistics of Sweden" pg 129"</t>
-  </si>
-  <si>
-    <t>NR</t>
   </si>
   <si>
     <t>21.5 
@@ -90,13 +87,13 @@
 (27.5 - 77.7)</t>
   </si>
   <si>
-    <t>Attack rate with asymptomatic per 100 (95% CI)</t>
-  </si>
-  <si>
-    <t>Cumulative attack rate per 100</t>
-  </si>
-  <si>
-    <t>Cumulative mortality rate per 100</t>
+    <t>Cumulative mortality (%)</t>
+  </si>
+  <si>
+    <t>Cumulative incidence (%)</t>
+  </si>
+  <si>
+    <t>Cumulative incidence with asymptomatic (%) [95% CI]</t>
   </si>
 </sst>
 </file>
@@ -225,7 +222,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -255,42 +252,26 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -668,7 +649,7 @@
         <v>3.4318626385568352</v>
       </c>
       <c r="H2" s="3">
-        <f>E2/D2</f>
+        <f t="shared" ref="H2:H8" si="0">E2/D2</f>
         <v>0.65618506718382053</v>
       </c>
       <c r="I2" s="11"/>
@@ -698,7 +679,7 @@
         <v>4.7442292077485213</v>
       </c>
       <c r="H3" s="5">
-        <f>E3/D3</f>
+        <f t="shared" si="0"/>
         <v>0.53886693017127796</v>
       </c>
       <c r="I3" s="11"/>
@@ -728,7 +709,7 @@
         <v>7.6805502483760026</v>
       </c>
       <c r="H4" s="23">
-        <f>E4/D4</f>
+        <f t="shared" si="0"/>
         <v>0.68367346938775508</v>
       </c>
       <c r="I4" s="24"/>
@@ -758,7 +739,7 @@
         <v>3.3270833333333334</v>
       </c>
       <c r="H5" s="14">
-        <f>E5/D5</f>
+        <f t="shared" si="0"/>
         <v>0.65103954341622505</v>
       </c>
       <c r="I5" s="11" t="s">
@@ -790,7 +771,7 @@
         <v>3.3526625285854297</v>
       </c>
       <c r="H6" s="14">
-        <f>E6/D6</f>
+        <f t="shared" si="0"/>
         <v>0.41538072350113836</v>
       </c>
       <c r="I6" s="11" t="s">
@@ -814,7 +795,7 @@
       <c r="F7" s="12"/>
       <c r="G7" s="13"/>
       <c r="H7" s="14">
-        <f>E7/D7</f>
+        <f t="shared" si="0"/>
         <v>0.39492002369668244</v>
       </c>
       <c r="I7" s="11"/>
@@ -844,7 +825,7 @@
         <v>9.2722798382844083</v>
       </c>
       <c r="H8" s="14">
-        <f>E8/D8</f>
+        <f t="shared" si="0"/>
         <v>0.54805194805194801</v>
       </c>
       <c r="I8" s="11" t="s">
@@ -867,72 +848,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.77734375" customWidth="1"/>
-    <col min="2" max="8" width="12.77734375" customWidth="1"/>
+    <col min="2" max="4" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="35.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="35.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2" s="27">
         <v>1853</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="27">
         <v>1853</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="27">
         <v>1857</v>
       </c>
-      <c r="E2" s="26">
-        <v>1853</v>
-      </c>
-      <c r="F2" s="26">
-        <v>1834</v>
-      </c>
-      <c r="G2" s="36">
-        <v>1852</v>
-      </c>
-      <c r="H2" s="26">
-        <v>1853</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="28">
@@ -944,21 +901,9 @@
       <c r="D3" s="28">
         <v>2617</v>
       </c>
-      <c r="E3" s="29">
-        <v>48000</v>
-      </c>
-      <c r="F3" s="25">
-        <v>97952</v>
-      </c>
-      <c r="G3" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="28">
-        <v>11378</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="28">
@@ -970,21 +915,9 @@
       <c r="D4" s="28">
         <v>294</v>
       </c>
-      <c r="E4" s="30">
-        <v>2453</v>
-      </c>
-      <c r="F4" s="25">
-        <v>7906</v>
-      </c>
-      <c r="G4" s="38">
-        <v>13504</v>
-      </c>
-      <c r="H4" s="25">
-        <v>1925</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="27" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="26" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="28">
@@ -996,156 +929,83 @@
       <c r="D5" s="28">
         <v>201</v>
       </c>
-      <c r="E5" s="30">
-        <v>1597</v>
-      </c>
-      <c r="F5" s="30">
-        <v>3284</v>
-      </c>
-      <c r="G5" s="38">
-        <v>5333</v>
-      </c>
-      <c r="H5" s="30">
-        <v>1055</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="31">
+    </row>
+    <row r="6" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="29">
         <f>B4/B3*100</f>
         <v>5.2300224588857498</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="29">
         <f>C4/C3*100</f>
         <v>8.8040830530100926</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="29">
         <f>D4/D3*100</f>
         <v>11.23423767672908</v>
       </c>
-      <c r="E6" s="31">
-        <f>E4/E3*100</f>
-        <v>5.1104166666666666</v>
-      </c>
-      <c r="F6" s="31">
-        <f>F4/F3*100</f>
-        <v>8.0713002286834374</v>
-      </c>
-      <c r="G6" s="39" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="31">
-        <f>H4/H3*100</f>
-        <v>16.918614870803307</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="35" t="s">
+      <c r="C7" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="D7" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="35" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="32"/>
-    </row>
-    <row r="8" spans="1:8" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="31">
+      <c r="B8" s="29">
         <f>B5/B3*100</f>
         <v>3.4318626385568352</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="29">
         <f>C5/C3*100</f>
         <v>4.7442292077485213</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="29">
         <f>D5/D3*100</f>
         <v>7.6805502483760026</v>
       </c>
-      <c r="E8" s="31">
-        <f>E5/E3*100</f>
-        <v>3.3270833333333334</v>
-      </c>
-      <c r="F8" s="31">
-        <f>F5/F3*100</f>
-        <v>3.3526625285854297</v>
-      </c>
-      <c r="G8" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="31">
-        <f>H5/H3*100</f>
-        <v>9.2722798382844083</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="27" t="s">
+    </row>
+    <row r="9" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="32">
-        <f>B5/B4</f>
+      <c r="B9" s="31">
+        <f t="shared" ref="B9:D9" si="0">B5/B4</f>
         <v>0.65618506718382053</v>
       </c>
-      <c r="C9" s="32">
-        <f>C5/C4</f>
+      <c r="C9" s="31">
+        <f t="shared" si="0"/>
         <v>0.53886693017127796</v>
       </c>
-      <c r="D9" s="32">
-        <f>D5/D4</f>
+      <c r="D9" s="31">
+        <f t="shared" si="0"/>
         <v>0.68367346938775508</v>
       </c>
-      <c r="E9" s="32">
-        <f>E5/E4</f>
-        <v>0.65103954341622505</v>
-      </c>
-      <c r="F9" s="32">
-        <f>F5/F4</f>
-        <v>0.41538072350113836</v>
-      </c>
-      <c r="G9" s="40">
-        <f>G5/G4</f>
-        <v>0.39492002369668244</v>
-      </c>
-      <c r="H9" s="32">
-        <f>H5/H4</f>
-        <v>0.54805194805194801</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25" t="s">
-        <v>16</v>
-      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>